<commit_message>
I have figured out the regex
</commit_message>
<xml_diff>
--- a/CH-126 Transformation.xlsx
+++ b/CH-126 Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1E21C9-330E-4873-8ED7-E280F16EF289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73121945-E1D6-4140-8D25-2D384D3E4898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Nice use of broadcasting</t>
+  </si>
+  <si>
+    <t>REGEXREPLACE(TEXT,pattern,replacement,occurrence,case_sensitivity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "([\/\d]+), ((?1)), ((?1))"</t>
+  </si>
+  <si>
+    <t>The ?1 means to refer back to the first capture group.</t>
   </si>
 </sst>
 </file>
@@ -2267,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EC0EF-4DDC-432E-8A0C-098C1F991CDC}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2674,6 +2683,9 @@
       <c r="D22" s="9">
         <v>45293</v>
       </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -2698,6 +2710,9 @@
       <c r="D24" s="9">
         <v>45303</v>
       </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="str">
@@ -2708,6 +2723,9 @@
       </c>
       <c r="D25" s="9">
         <v>45298</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2878,8 +2896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB906E4-F4ED-4118-9939-02F75E883835}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on using implicit intersection
</commit_message>
<xml_diff>
--- a/CH-126 Transformation.xlsx
+++ b/CH-126 Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73121945-E1D6-4140-8D25-2D384D3E4898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13830618-3B34-4175-BFA1-94AA3E036804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="37">
   <si>
     <t>Question</t>
   </si>
@@ -142,6 +142,42 @@
   </si>
   <si>
     <t>The ?1 means to refer back to the first capture group.</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>zz</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>ww</t>
   </si>
 </sst>
 </file>
@@ -465,6 +501,7 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,7 +514,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -1351,15 +1387,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1780,15 +1816,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -2276,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EC0EF-4DDC-432E-8A0C-098C1F991CDC}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2292,15 +2328,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -2894,10 +2930,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB906E4-F4ED-4118-9939-02F75E883835}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2913,15 +2949,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="E1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -3278,7 +3314,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="23" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3480,7 +3516,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E33" s="5" t="str">
         <v>O004</v>
       </c>
@@ -3491,7 +3527,7 @@
         <v>45312</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E34" s="5" t="str">
         <v>O004</v>
       </c>
@@ -3502,7 +3538,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E35" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3513,7 +3549,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E36" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3524,7 +3560,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E37" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3535,7 +3571,7 @@
         <v>45313</v>
       </c>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E38" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3546,7 +3582,7 @@
         <v>45297</v>
       </c>
     </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E39" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3557,7 +3593,7 @@
         <v>45299</v>
       </c>
     </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E40" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3566,6 +3602,133 @@
       </c>
       <c r="G40" s="5">
         <v>45305</v>
+      </c>
+    </row>
+    <row r="41" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" t="s">
+        <v>26</v>
+      </c>
+      <c r="M41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" t="s">
+        <v>28</v>
+      </c>
+      <c r="L42" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" t="s">
+        <v>31</v>
+      </c>
+      <c r="L43" t="s">
+        <v>32</v>
+      </c>
+      <c r="M43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J45" t="str" cm="1">
+        <f t="array" ref="J45:L47">_xlfn.SINGLE(+J41:J43)&amp;K41:M43</f>
+        <v>zza</v>
+      </c>
+      <c r="K45" t="str">
+        <v>zzb</v>
+      </c>
+      <c r="L45" t="str">
+        <v>zzc</v>
+      </c>
+    </row>
+    <row r="46" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J46" t="str">
+        <v>zzd</v>
+      </c>
+      <c r="K46" t="str">
+        <v>zze</v>
+      </c>
+      <c r="L46" t="str">
+        <v>zzf</v>
+      </c>
+    </row>
+    <row r="47" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J47" t="str">
+        <v>zzg</v>
+      </c>
+      <c r="K47" t="str">
+        <v>zzh</v>
+      </c>
+      <c r="L47" t="str">
+        <v>zzi</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" t="str" cm="1">
+        <f t="array" ref="H49:H58">_xlfn.REDUCE("",K41:M43,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.SINGLE(+J43:_xlpm.v)&amp;_xlpm.v)))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" t="str">
+        <v>zza</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" t="str">
+        <v>zzb</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H52" t="str">
+        <v>zzc</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H53" t="str">
+        <v>yyd</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54" t="str">
+        <v>yye</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H55" t="str">
+        <v>yyf</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H56" t="str">
+        <v>wwg</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57" t="str">
+        <v>wwh</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H58" t="str">
+        <v>wwi</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I established what this exercise taught me
</commit_message>
<xml_diff>
--- a/CH-126 Transformation.xlsx
+++ b/CH-126 Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13830618-3B34-4175-BFA1-94AA3E036804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5929D-2DAA-4E85-A9CC-AF350DA4D324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="42">
   <si>
     <t>Question</t>
   </si>
@@ -178,13 +178,28 @@
   </si>
   <si>
     <t>ww</t>
+  </si>
+  <si>
+    <t>This is what was done to repeat the front number</t>
+  </si>
+  <si>
+    <t>What did I master in this drill?</t>
+  </si>
+  <si>
+    <t>I finally figure out how to use the intersect operator to fill a column</t>
+  </si>
+  <si>
+    <t>I see that the instance parameter can be an array</t>
+  </si>
+  <si>
+    <t>You can use broadcasting to repeat a string across variables.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +241,13 @@
       <name val="Aptos Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -441,11 +463,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -514,9 +537,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1800,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677DA5E6-B2FD-4CAC-B9CE-06B03CBA8953}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2930,10 +2957,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB906E4-F4ED-4118-9939-02F75E883835}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3516,7 +3543,7 @@
         <v>45310</v>
       </c>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E33" s="5" t="str">
         <v>O004</v>
       </c>
@@ -3527,7 +3554,7 @@
         <v>45312</v>
       </c>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E34" s="5" t="str">
         <v>O004</v>
       </c>
@@ -3538,7 +3565,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E35" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3549,7 +3576,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E36" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3560,7 +3587,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E37" s="5" t="str">
         <v>O005</v>
       </c>
@@ -3571,7 +3598,7 @@
         <v>45313</v>
       </c>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E38" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3582,7 +3609,7 @@
         <v>45297</v>
       </c>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E39" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3593,7 +3620,7 @@
         <v>45299</v>
       </c>
     </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E40" s="5" t="str">
         <v>O006</v>
       </c>
@@ -3604,7 +3631,7 @@
         <v>45305</v>
       </c>
     </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>34</v>
       </c>
@@ -3618,7 +3645,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B42" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="J42" t="s">
         <v>35</v>
       </c>
@@ -3632,7 +3662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
         <v>36</v>
       </c>
@@ -3646,7 +3676,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
       <c r="J45" t="str" cm="1">
         <f t="array" ref="J45:L47">_xlfn.SINGLE(+J41:J43)&amp;K41:M43</f>
         <v>zza</v>
@@ -3658,7 +3702,13 @@
         <v>zzc</v>
       </c>
     </row>
-    <row r="46" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
       <c r="J46" t="str">
         <v>zzd</v>
       </c>
@@ -3669,7 +3719,7 @@
         <v>zzf</v>
       </c>
     </row>
-    <row r="47" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J47" t="str">
         <v>zzg</v>
       </c>
@@ -3680,55 +3730,90 @@
         <v>zzi</v>
       </c>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" t="str" cm="1">
-        <f t="array" ref="H49:H58">_xlfn.REDUCE("",K41:M43,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.SINGLE(+J43:_xlpm.v)&amp;_xlpm.v)))</f>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H51" t="str" cm="1">
+        <f t="array" ref="H51:I60">_xlfn.REDUCE("",K41:M43,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlfn.SINGLE(+J43:_xlpm.v)&amp;"|"&amp;_xlpm.v,"|"))))</f>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" t="str">
-        <v>zza</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" t="str">
-        <v>zzb</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H52" t="str">
-        <v>zzc</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+        <v>zz</v>
+      </c>
+      <c r="I52" t="str">
+        <v>a</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H53" t="str">
-        <v>yyd</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+        <v>zz</v>
+      </c>
+      <c r="I53" t="str">
+        <v>b</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H54" t="str">
-        <v>yye</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+        <v>zz</v>
+      </c>
+      <c r="I54" t="str">
+        <v>c</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H55" t="str">
-        <v>yyf</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+        <v>yy</v>
+      </c>
+      <c r="I55" t="str">
+        <v>d</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H56" t="str">
-        <v>wwg</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+        <v>yy</v>
+      </c>
+      <c r="I56" t="str">
+        <v>e</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H57" t="str">
-        <v>wwh</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+        <v>yy</v>
+      </c>
+      <c r="I57" t="str">
+        <v>f</v>
+      </c>
+    </row>
+    <row r="58" spans="6:9" x14ac:dyDescent="0.25">
       <c r="H58" t="str">
-        <v>wwi</v>
+        <v>ww</v>
+      </c>
+      <c r="I58" t="str">
+        <v>g</v>
+      </c>
+    </row>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H59" t="str">
+        <v>ww</v>
+      </c>
+      <c r="I59" t="str">
+        <v>h</v>
+      </c>
+    </row>
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H60" t="str">
+        <v>ww</v>
+      </c>
+      <c r="I60" t="str">
+        <v>i</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on standard method for converting a table to long form
</commit_message>
<xml_diff>
--- a/CH-126 Transformation.xlsx
+++ b/CH-126 Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5929D-2DAA-4E85-A9CC-AF350DA4D324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B85592-3926-439C-9D1E-E47D2F1FA251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="43">
   <si>
     <t>Question</t>
   </si>
@@ -194,6 +194,9 @@
   <si>
     <t>You can use broadcasting to repeat a string across variables.</t>
   </si>
+  <si>
+    <t>Registration</t>
+  </si>
 </sst>
 </file>
 
@@ -525,6 +528,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -536,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1414,15 +1417,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="E1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1825,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677DA5E6-B2FD-4CAC-B9CE-06B03CBA8953}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1840,18 +1843,20 @@
     <col min="5" max="5" width="14.59765625" style="5" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="11.19921875" customWidth="1"/>
+    <col min="9" max="9" width="12.796875" customWidth="1"/>
+    <col min="10" max="10" width="12.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="E1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1886,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G3" s="16">
         <v>45293</v>
@@ -1955,7 +1960,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G6" s="16">
         <v>45298</v>
@@ -2015,7 +2020,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G9" s="16">
         <v>45300</v>
@@ -2069,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G12" s="16">
         <v>45310</v>
@@ -2118,7 +2123,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G15" s="16">
         <v>45294</v>
@@ -2140,7 +2145,7 @@
         <v>45296</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2156,7 +2161,7 @@
       </c>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -2165,14 +2170,14 @@
         <v>10</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G18" s="16">
         <v>45297</v>
       </c>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2187,7 +2192,7 @@
         <v>45299</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2203,13 +2208,13 @@
       </c>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9" t="str" cm="1">
@@ -2228,9 +2233,32 @@
         <f ca="1"/>
         <v>2024/01/12</v>
       </c>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22:H39">_xlfn.TOCOL(_xlfn.DROP(_xlfn.REDUCE("",REPT(C22:C27&amp;"|",3),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1,-1))</f>
+        <v>O001</v>
+      </c>
+      <c r="I22" t="str" cm="1">
+        <f t="array" ref="I22:I39">_xlfn.REDUCE({"Registration";"Evaluation";"Approved"},_xlfn.SEQUENCE(5),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TAKE(_xlpm.a,3))))</f>
+        <v>Registration</v>
+      </c>
+      <c r="J22" s="16" cm="1">
+        <f t="array" aca="1" ref="J22:J39" ca="1">_xlfn.TOCOL(D22:F27)+0</f>
+        <v>45293</v>
+      </c>
+      <c r="L22" t="b" cm="1">
+        <f t="array" aca="1" ref="L22:N39" ca="1">H22:J39=E3:G20</f>
+        <v>1</v>
+      </c>
+      <c r="M22" s="2" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N22" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9" t="str">
@@ -2249,8 +2277,30 @@
         <f ca="1"/>
         <v>2024/01/15</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <v>O001</v>
+      </c>
+      <c r="I23" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J23" s="16">
+        <f ca="1"/>
+        <v>45301</v>
+      </c>
+      <c r="L23" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N23" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="str">
         <f ca="1"/>
@@ -2268,8 +2318,30 @@
         <f ca="1"/>
         <v>2024/01/23</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <v>O001</v>
+      </c>
+      <c r="I24" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J24" s="16">
+        <f ca="1"/>
+        <v>45303</v>
+      </c>
+      <c r="L24" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N24" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="str">
         <f ca="1"/>
@@ -2287,8 +2359,30 @@
         <f ca="1"/>
         <v>2024/01/24</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <v>O002</v>
+      </c>
+      <c r="I25" t="str">
+        <v>Registration</v>
+      </c>
+      <c r="J25" s="16">
+        <f ca="1"/>
+        <v>45298</v>
+      </c>
+      <c r="L25" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N25" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9" t="str">
         <f ca="1"/>
@@ -2306,8 +2400,30 @@
         <f ca="1"/>
         <v>2024/01/22</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <v>O002</v>
+      </c>
+      <c r="I26" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J26" s="16">
+        <f ca="1"/>
+        <v>45304</v>
+      </c>
+      <c r="L26" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N26" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27" s="9" t="str">
         <f ca="1"/>
         <v>O006</v>
@@ -2323,6 +2439,316 @@
       <c r="F27" s="9" t="str">
         <f ca="1"/>
         <v>2024/01/14</v>
+      </c>
+      <c r="H27" t="str">
+        <v>O002</v>
+      </c>
+      <c r="I27" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J27" s="16">
+        <f ca="1"/>
+        <v>45306</v>
+      </c>
+      <c r="L27" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N27" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <v>O003</v>
+      </c>
+      <c r="I28" t="str">
+        <v>Registration</v>
+      </c>
+      <c r="J28" s="16">
+        <f ca="1"/>
+        <v>45300</v>
+      </c>
+      <c r="L28" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N28" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <v>O003</v>
+      </c>
+      <c r="I29" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J29" s="16">
+        <f ca="1"/>
+        <v>45307</v>
+      </c>
+      <c r="L29" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M29" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <v>O003</v>
+      </c>
+      <c r="I30" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J30" s="16">
+        <f ca="1"/>
+        <v>45314</v>
+      </c>
+      <c r="L30" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N30" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <v>O004</v>
+      </c>
+      <c r="I31" t="str">
+        <v>Registration</v>
+      </c>
+      <c r="J31" s="16">
+        <f ca="1"/>
+        <v>45310</v>
+      </c>
+      <c r="L31" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N31" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <v>O004</v>
+      </c>
+      <c r="I32" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J32" s="16">
+        <f ca="1"/>
+        <v>45312</v>
+      </c>
+      <c r="L32" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M32" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N32" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <v>O004</v>
+      </c>
+      <c r="I33" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J33" s="16">
+        <f ca="1"/>
+        <v>45315</v>
+      </c>
+      <c r="L33" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M33" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N33" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <v>O005</v>
+      </c>
+      <c r="I34" t="str">
+        <v>Registration</v>
+      </c>
+      <c r="J34" s="16">
+        <f ca="1"/>
+        <v>45294</v>
+      </c>
+      <c r="L34" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M34" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N34" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <v>O005</v>
+      </c>
+      <c r="I35" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J35" s="16">
+        <f ca="1"/>
+        <v>45296</v>
+      </c>
+      <c r="L35" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N35" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <v>O005</v>
+      </c>
+      <c r="I36" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J36" s="16">
+        <f ca="1"/>
+        <v>45313</v>
+      </c>
+      <c r="L36" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N36" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <v>O006</v>
+      </c>
+      <c r="I37" t="str">
+        <v>Registration</v>
+      </c>
+      <c r="J37" s="16">
+        <f ca="1"/>
+        <v>45297</v>
+      </c>
+      <c r="L37" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M37" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N37" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H38" t="str">
+        <v>O006</v>
+      </c>
+      <c r="I38" t="str">
+        <v>Evaluation</v>
+      </c>
+      <c r="J38" s="16">
+        <f ca="1"/>
+        <v>45299</v>
+      </c>
+      <c r="L38" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N38" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <v>O006</v>
+      </c>
+      <c r="I39" t="str">
+        <v>Approved</v>
+      </c>
+      <c r="J39" s="19">
+        <f ca="1"/>
+        <v>45305</v>
+      </c>
+      <c r="L39" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M39" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N39" t="b">
+        <f ca="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2339,8 +2765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5EC0EF-4DDC-432E-8A0C-098C1F991CDC}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="C24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="C17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2355,15 +2781,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="E1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -2959,8 +3385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB906E4-F4ED-4118-9939-02F75E883835}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2976,15 +3402,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="E1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
@@ -3646,7 +4072,7 @@
       </c>
     </row>
     <row r="42" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="24" t="s">
         <v>38</v>
       </c>
       <c r="J42" t="s">

</xml_diff>

<commit_message>
I think I am done
</commit_message>
<xml_diff>
--- a/CH-126 Transformation.xlsx
+++ b/CH-126 Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8715AD-4052-4111-8C6D-92C4A8591716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48376F-3FD8-4BE6-A953-EFD09474257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="45">
   <si>
     <t>Question</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Registration</t>
+  </si>
+  <si>
+    <t>Repeat command</t>
+  </si>
+  <si>
+    <t>Stack command</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1837,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2213,6 +2219,9 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
+      <c r="I21" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -2515,6 +2524,9 @@
       <c r="C30" t="str" cm="1">
         <f t="array" aca="1" ref="C30:C47" ca="1">_xlfn.TOCOL(_xlfn.DROP(_xlfn.REDUCE("",C22:C27,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MID(REPT(_xlpm.v,3),{1,5,9},4)))),1))</f>
         <v>O001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
       </c>
       <c r="H30" t="str">
         <v>O003</v>

</xml_diff>